<commit_message>
pending office 365 innozant
</commit_message>
<xml_diff>
--- a/INNOZANT/ALL_PRACTICE_FILES/OFFICE 365/19.Excel xlookup function.xlsx
+++ b/INNOZANT/ALL_PRACTICE_FILES/OFFICE 365/19.Excel xlookup function.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\innozant\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\Excel\INNOZANT\ALL_PRACTICE_FILES\OFFICE 365\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA46B18-1C43-4341-87A5-D0FD454DF11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39EAC8E-705D-46D9-B4A5-85C2B184692F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="9" xr2:uid="{D17EF5F1-9051-463C-B9C6-06B31CB2551C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D17EF5F1-9051-463C-B9C6-06B31CB2551C}"/>
   </bookViews>
   <sheets>
     <sheet name="Vertical XLOOKUP" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -272,7 +272,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,13 +300,6 @@
       <color indexed="12"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="8"/>
@@ -339,21 +332,41 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,27 +381,40 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
+        <fgColor indexed="30"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -404,17 +430,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="2" tint="-0.499984740745262"/>
@@ -423,15 +438,6 @@
       <bottom style="thin">
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -446,50 +452,10 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="thin">
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -499,17 +465,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -525,23 +480,38 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
+        <color indexed="22"/>
       </left>
       <right style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
+        <color indexed="22"/>
       </right>
       <top style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
+        <color indexed="22"/>
       </left>
       <right style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
+        <color indexed="22"/>
       </right>
       <top/>
       <bottom/>
@@ -549,32 +519,29 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
+        <color indexed="22"/>
       </left>
       <right style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
+        <color indexed="22"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
+        <color indexed="22"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color indexed="22"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color indexed="22"/>
       </bottom>
       <diagonal/>
     </border>
@@ -586,209 +553,105 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -813,9 +676,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -853,7 +716,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -959,7 +822,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1101,7 +964,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1109,81 +972,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB431B64-3EAC-41EC-BE7D-63CC3BFDF35E}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="13">
         <v>3970</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="4" cm="1">
+      <c r="E2" s="13" cm="1">
         <f t="array" ref="E2">_xlfn.XLOOKUP(E1, A2:A6, B2:B6)</f>
         <v>3741</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="13">
         <v>3646</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="13">
         <v>3741</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="13">
         <v>3270</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="13">
         <v>1205</v>
       </c>
     </row>
@@ -1195,81 +1054,78 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE59B445-7E61-463D-AFE8-7A9FD2C05171}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView showGridLines="0" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="34" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="24">
         <v>19528</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="4" t="str">
+      <c r="E2" s="1" t="str">
         <f>_xlfn.XLOOKUP(E1, A2:A6, B2:B6, "No match is found")</f>
         <v>No match is found</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="24">
         <v>23408</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="24">
         <v>22936</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="24">
         <v>16852</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="24">
         <v>19805</v>
       </c>
     </row>
@@ -1283,66 +1139,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FE4184-8A01-42DF-9EF2-985A7D58E01C}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView showGridLines="0" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="12">
         <v>3970</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="12">
         <v>3646</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="12">
         <v>3741</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="12">
         <v>3270</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="12">
         <v>1205</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="4" cm="1">
+      <c r="I2" s="12" cm="1">
         <f t="array" ref="I2">_xlfn.XLOOKUP(I1, B1:F1, B2:F2)</f>
         <v>3741</v>
       </c>
@@ -1355,99 +1211,96 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB36D27A-F7E3-4B95-89FB-8750ACCA6686}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="13">
         <v>3970</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4" cm="1">
+      <c r="F2" s="12" cm="1">
         <f t="array" ref="F2">_xlfn.XLOOKUP(F1, B2:B6, A2:A6)</f>
         <v>3</v>
       </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="13">
         <v>3646</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="13">
         <v>3741</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="13">
         <v>3270</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="13">
         <v>1205</v>
       </c>
     </row>
@@ -1461,265 +1314,265 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2EB6D3-9727-46B4-B073-E95EA42D5504}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+    <col min="5" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="58" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="15">
+      <c r="A3" s="18"/>
+      <c r="B3" s="12">
         <v>90</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="12">
         <v>98</v>
       </c>
-      <c r="G3" s="26" t="str">
+      <c r="G3" s="12" t="str">
         <f>_xlfn.XLOOKUP(F3, $B$3:$B$7, $C$3:$C$7, ,-1)</f>
         <v>A</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="15">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="12">
         <v>80</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="12">
         <v>60</v>
       </c>
-      <c r="G4" s="26" t="str">
+      <c r="G4" s="12" t="str">
         <f t="shared" ref="G4:G7" si="0">_xlfn.XLOOKUP(F4, $B$3:$B$7, $C$3:$C$7, ,-1)</f>
         <v>D</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="15">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="12">
         <v>70</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="12">
         <v>48</v>
       </c>
-      <c r="G5" s="26" t="str">
+      <c r="G5" s="12" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
-      <c r="B6" s="15">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="12">
         <v>60</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="12">
         <v>71</v>
       </c>
-      <c r="G6" s="26" t="str">
+      <c r="G6" s="12" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="90"/>
-      <c r="B7" s="25">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="12">
         <v>0</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="12">
         <v>82</v>
       </c>
-      <c r="G7" s="26" t="str">
+      <c r="G7" s="12" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="58" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="58" t="s">
+      <c r="F11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="89" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="24">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="12">
         <v>59</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="12">
         <v>98</v>
       </c>
-      <c r="G12" s="26" t="str">
+      <c r="G12" s="12" t="str">
         <f>_xlfn.XLOOKUP(F12, $B$12:$B$16, $C$12:$C$16, ,1)</f>
         <v>A</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="89"/>
-      <c r="B13" s="15">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="12">
         <v>69</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="12">
         <v>60</v>
       </c>
-      <c r="G13" s="26" t="str">
+      <c r="G13" s="12" t="str">
         <f t="shared" ref="G13:G16" si="1">_xlfn.XLOOKUP(F13, $B$12:$B$16, $C$12:$C$16, ,1)</f>
         <v>D</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="89"/>
-      <c r="B14" s="15">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="12">
         <v>79</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="12">
         <v>48</v>
       </c>
-      <c r="G14" s="26" t="str">
+      <c r="G14" s="12" t="str">
         <f t="shared" si="1"/>
         <v>F</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="89"/>
-      <c r="B15" s="15">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="12">
         <v>89</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="12">
         <v>71</v>
       </c>
-      <c r="G15" s="26" t="str">
+      <c r="G15" s="12" t="str">
         <f t="shared" si="1"/>
         <v>C</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="90"/>
-      <c r="B16" s="16">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="12">
         <v>100</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="12">
         <v>82</v>
       </c>
-      <c r="G16" s="28" t="str">
+      <c r="G16" s="12" t="str">
         <f t="shared" si="1"/>
         <v>B</v>
       </c>
@@ -1729,10 +1582,10 @@
     <sortCondition descending="1" ref="B3"/>
   </sortState>
   <mergeCells count="4">
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A12:A16"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A11:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1743,91 +1596,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568F55FE-8DAF-468E-8154-1F145435D46B}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="12">
         <v>22023</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="12">
         <f>_xlfn.XLOOKUP("*"&amp;E1&amp;"*", A2:A8, B2:B8, ,2)</f>
         <v>19008</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="12">
         <v>19008</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="12">
         <v>23707</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="12">
         <v>17171</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="12">
         <v>19754</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="12">
         <v>16925</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="12">
         <v>18470</v>
       </c>
     </row>
@@ -1841,157 +1693,157 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C585EEFF-0DE0-4E4E-BBCB-B5480BCAFD51}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="1" max="4" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="83" t="s">
+      <c r="C1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="33">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
         <v>44440</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="61">
+      <c r="D2" s="13">
         <v>15389</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="62">
+      <c r="G2" s="12">
         <f>_xlfn.XLOOKUP(G1, B2:B9, D2:D9, , ,-1)</f>
         <v>15592</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="33">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
         <v>44441</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="61">
+      <c r="D3" s="13">
         <v>17111</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
         <v>44442</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="61">
+      <c r="D4" s="13">
         <v>14802</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="33">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
         <v>44443</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="61">
+      <c r="D5" s="13">
         <v>10757</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
         <v>44444</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="13">
         <v>15592</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="33">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
         <v>44445</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="61">
+      <c r="D7" s="13">
         <v>15785</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="33">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
         <v>44446</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="61">
+      <c r="D8" s="13">
         <v>18281</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="33">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
         <v>44447</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="13">
         <v>19007</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1999,214 +1851,206 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80819A05-F824-4C5A-8A61-652E38CBDD5E}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="K1" s="51" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="K1" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="80" t="s">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="59" t="s">
+      <c r="I2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="K2" s="27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="64" t="s">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="23">
         <v>44440</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="65">
+      <c r="D3" s="24">
         <v>15389</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="37" cm="1">
+      <c r="G3" s="23" cm="1">
         <f t="array" ref="G3:I3">_xlfn.XLOOKUP(F3, A3:A8, B3:D8)</f>
         <v>44443</v>
       </c>
-      <c r="H3" s="16" t="str">
+      <c r="H3" s="22" t="str">
         <v>Samsung</v>
       </c>
-      <c r="I3" s="35">
+      <c r="I3" s="26">
         <v>10757</v>
       </c>
-      <c r="K3" s="41" cm="1">
+      <c r="K3" s="26" cm="1">
         <f t="array" ref="K3:K8">_xlfn.XLOOKUP(K2, A2:D2, A3:D8)</f>
         <v>15389</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="23">
         <v>44441</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="65">
+      <c r="D4" s="24">
         <v>17111</v>
       </c>
-      <c r="K4" s="41">
+      <c r="K4" s="26">
         <v>17111</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="23">
         <v>44442</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="65">
+      <c r="D5" s="24">
         <v>14802</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="41">
+      <c r="K5" s="26">
         <v>14802</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="23">
         <v>44443</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="65">
+      <c r="D6" s="24">
         <v>10757</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="38" cm="1">
+      <c r="G6" s="3" cm="1">
         <f t="array" ref="G6:G8">TRANSPOSE(_xlfn.XLOOKUP(G5, A3:A8, B3:D8))</f>
         <v>44444</v>
       </c>
-      <c r="K6" s="41">
+      <c r="K6" s="26">
         <v>10757</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="66" t="s">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="23">
         <v>44444</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="65">
+      <c r="D7" s="24">
         <v>15592</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="39" t="str">
+      <c r="G7" s="4" t="str">
         <v>Nokia</v>
       </c>
-      <c r="K7" s="41">
+      <c r="K7" s="26">
         <v>15592</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="68">
+      <c r="B8" s="23">
         <v>44445</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="70">
+      <c r="D8" s="24">
         <v>15785</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="F8" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="5">
         <v>15592</v>
       </c>
-      <c r="K8" s="42">
+      <c r="K8" s="26">
         <v>15785</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="63"/>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="63"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
+      <c r="D10" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2221,180 +2065,180 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E0D56C-098C-4DB4-8420-FE3B40DF5629}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="1" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="48">
+      <c r="G1" s="29">
         <v>44441</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="71">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23">
         <v>44440</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="75">
+      <c r="D2" s="24">
         <v>12836</v>
       </c>
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="71">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23">
         <v>44440</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="75">
+      <c r="D3" s="24">
         <v>12017</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="71">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
         <v>44440</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="75">
+      <c r="D4" s="24">
         <v>15461</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="10" cm="1">
+      <c r="G4" s="31" cm="1">
         <f t="array" ref="G4">_xlfn.XLOOKUP(1, (A2:A10=G1) * (B2:B10=G2) * (C2:C10=G3), D2:D10)</f>
         <v>14054</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="71">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23">
         <v>44440</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="75">
+      <c r="D5" s="24">
         <v>12515</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="71">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
         <v>44440</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="75">
+      <c r="D6" s="24">
         <v>18880</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="71">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23">
         <v>44441</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="75">
+      <c r="D7" s="24">
         <v>10929</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="71">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
         <v>44441</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="75">
+      <c r="D8" s="24">
         <v>14634</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="71">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23">
         <v>44441</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="24">
         <v>14054</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="72">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23">
         <v>44441</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="76">
+      <c r="D10" s="24">
         <v>14371</v>
       </c>
     </row>
@@ -2408,137 +2252,137 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0DD3CE-2BF7-4EF1-A9EC-890398F08637}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="1" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="87">
+      <c r="B2" s="24">
         <v>775</v>
       </c>
-      <c r="C2" s="87">
+      <c r="C2" s="24">
         <v>592</v>
       </c>
-      <c r="D2" s="87">
+      <c r="D2" s="24">
         <v>793</v>
       </c>
-      <c r="E2" s="61">
+      <c r="E2" s="24">
         <v>804</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="87">
+      <c r="B3" s="24">
         <v>821</v>
       </c>
-      <c r="C3" s="87">
+      <c r="C3" s="24">
         <v>626</v>
       </c>
-      <c r="D3" s="87">
+      <c r="D3" s="24">
         <v>720</v>
       </c>
-      <c r="E3" s="61">
+      <c r="E3" s="24">
         <v>750</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="10" cm="1">
+      <c r="H3" s="2" cm="1">
         <f t="array" ref="H3">_xlfn.XLOOKUP(H1, A2:A6, _xlfn.XLOOKUP(H2, B1:E1, B2:E6))</f>
         <v>626</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="87">
+      <c r="B4" s="24">
         <v>680</v>
       </c>
-      <c r="C4" s="87">
+      <c r="C4" s="24">
         <v>778</v>
       </c>
-      <c r="D4" s="87">
+      <c r="D4" s="24">
         <v>983</v>
       </c>
-      <c r="E4" s="61">
+      <c r="E4" s="24">
         <v>598</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="87">
+      <c r="B5" s="24">
         <v>556</v>
       </c>
-      <c r="C5" s="87">
+      <c r="C5" s="24">
         <v>681</v>
       </c>
-      <c r="D5" s="87">
+      <c r="D5" s="24">
         <v>698</v>
       </c>
-      <c r="E5" s="61">
+      <c r="E5" s="24">
         <v>635</v>
       </c>
-      <c r="F5" s="53"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="88">
+      <c r="B6" s="24">
         <v>581</v>
       </c>
-      <c r="C6" s="88">
+      <c r="C6" s="24">
         <v>650</v>
       </c>
-      <c r="D6" s="88">
+      <c r="D6" s="24">
         <v>689</v>
       </c>
-      <c r="E6" s="62">
+      <c r="E6" s="24">
         <v>520</v>
       </c>
     </row>

</xml_diff>